<commit_message>
- fix unit bonuses
</commit_message>
<xml_diff>
--- a/output/spreadsheets/12.04/sends.xlsx
+++ b/output/spreadsheets/12.04/sends.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG40"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2743,7 +2743,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hydralisk</t>
+          <t>Ghost</t>
         </is>
       </c>
       <c r="B21">
@@ -2767,16 +2767,16 @@
         <v/>
       </c>
       <c r="G21" t="n">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="H21" t="n">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="I21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J21" t="n">
-        <v>12.5</v>
+        <v>12.25</v>
       </c>
       <c r="K21">
         <f>E21/G21</f>
@@ -2793,7 +2793,7 @@
         <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="P21" t="n">
         <v>1</v>
@@ -2808,45 +2808,45 @@
         <v>1</v>
       </c>
       <c r="T21" t="n">
-        <v>653</v>
+        <v>575</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>Armored</t>
+          <t>Light</t>
         </is>
       </c>
       <c r="W21" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>Piercing</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="Y21" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="Z21" t="n">
         <v>1</v>
       </c>
       <c r="AA21" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="AB21" t="n">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="AC21" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AD21" t="n">
         <v>2.5</v>
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>Target attacks 20% slower and takes 45 damage over 3 seconds (does not stack)</t>
+          <t>Detonates an EMP at target point that strips 100.00 + 5.00% shields from enemies.</t>
         </is>
       </c>
       <c r="AF21" t="inlineStr"/>
@@ -2855,7 +2855,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Queen</t>
+          <t>Hydralisk</t>
         </is>
       </c>
       <c r="B22">
@@ -2905,7 +2905,7 @@
         <v>1</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="P22" t="n">
         <v>1</v>
@@ -2920,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="T22" t="n">
-        <v>676</v>
+        <v>653</v>
       </c>
       <c r="U22" t="n">
         <v>0</v>
@@ -2935,30 +2935,30 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Piercing</t>
         </is>
       </c>
       <c r="Y22" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Z22" t="n">
         <v>1</v>
       </c>
       <c r="AA22" t="n">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="AB22" t="n">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AD22" t="n">
         <v>2.5</v>
       </c>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>Slows enemies in 6.5 range by 40.00% (does not stack)</t>
+          <t>Target attacks 20% slower and takes 45 damage over 3 seconds (does not stack)</t>
         </is>
       </c>
       <c r="AF22" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Aberration Basher</t>
+          <t>Queen</t>
         </is>
       </c>
       <c r="B23">
@@ -2991,16 +2991,16 @@
         <v/>
       </c>
       <c r="G23" t="n">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="H23" t="n">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="I23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J23" t="n">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="K23">
         <f>E23/G23</f>
@@ -3014,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>1.18</v>
+        <v>1</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -3032,14 +3032,14 @@
         <v>1</v>
       </c>
       <c r="T23" t="n">
-        <v>378</v>
+        <v>676</v>
       </c>
       <c r="U23" t="n">
         <v>0</v>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Armored</t>
         </is>
       </c>
       <c r="W23" t="n">
@@ -3047,30 +3047,30 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>Siege</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="Y23" t="n">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="Z23" t="n">
         <v>1</v>
       </c>
       <c r="AA23" t="n">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="AB23" t="n">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="AC23" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="AD23" t="n">
         <v>2.5</v>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>Allies gain 20.00% damage reduction (does not stack)</t>
+          <t>Slows enemies in 6.5 range by 40.00% (does not stack)</t>
         </is>
       </c>
       <c r="AF23" t="inlineStr"/>
@@ -3079,7 +3079,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Dark Templar</t>
+          <t>Aberration Basher</t>
         </is>
       </c>
       <c r="B24">
@@ -3106,13 +3106,13 @@
         <v>360</v>
       </c>
       <c r="H24" t="n">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="I24" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J24" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K24">
         <f>E24/G24</f>
@@ -3126,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>1</v>
+        <v>1.18</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
@@ -3144,14 +3144,14 @@
         <v>1</v>
       </c>
       <c r="T24" t="n">
-        <v>941</v>
+        <v>378</v>
       </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>Armored</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W24" t="n">
@@ -3159,30 +3159,30 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Siege</t>
         </is>
       </c>
       <c r="Y24" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="Z24" t="n">
         <v>1</v>
       </c>
       <c r="AA24" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AB24" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="AD24" t="n">
         <v>2.5</v>
       </c>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>Nearby allies move 20% faster (does not stack)</t>
+          <t>Allies gain 20.00% damage reduction (does not stack)</t>
         </is>
       </c>
       <c r="AF24" t="inlineStr"/>
@@ -3191,7 +3191,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Powermortal</t>
+          <t>Dark Templar</t>
         </is>
       </c>
       <c r="B25">
@@ -3215,13 +3215,13 @@
         <v/>
       </c>
       <c r="G25" t="n">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="H25" t="n">
         <v>300</v>
       </c>
       <c r="I25" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J25" t="n">
         <v>15</v>
@@ -3235,7 +3235,7 @@
         <v/>
       </c>
       <c r="M25" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
         <v>1</v>
@@ -3256,14 +3256,14 @@
         <v>1</v>
       </c>
       <c r="T25" t="n">
-        <v>826</v>
+        <v>941</v>
       </c>
       <c r="U25" t="n">
         <v>0</v>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Armored</t>
         </is>
       </c>
       <c r="W25" t="n">
@@ -3281,33 +3281,29 @@
         <v>1</v>
       </c>
       <c r="AA25" t="n">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="AB25" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="AC25" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AD25" t="n">
         <v>2.5</v>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>Rapidly regenerates life</t>
-        </is>
-      </c>
-      <c r="AF25" t="inlineStr">
-        <is>
-          <t>Gives ideal income for the cost</t>
-        </is>
-      </c>
+          <t>Nearby allies move 20% faster (does not stack)</t>
+        </is>
+      </c>
+      <c r="AF25" t="inlineStr"/>
       <c r="AG25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Hellion</t>
+          <t>Powermortal</t>
         </is>
       </c>
       <c r="B26">
@@ -3331,13 +3327,13 @@
         <v/>
       </c>
       <c r="G26" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H26" t="n">
         <v>300</v>
       </c>
       <c r="I26" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J26" t="n">
         <v>15</v>
@@ -3351,7 +3347,7 @@
         <v/>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N26" t="n">
         <v>1</v>
@@ -3360,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
@@ -3372,14 +3368,14 @@
         <v>1</v>
       </c>
       <c r="T26" t="n">
-        <v>735</v>
+        <v>826</v>
       </c>
       <c r="U26" t="n">
         <v>0</v>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>Light</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W26" t="n">
@@ -3387,39 +3383,43 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>Magic</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="Y26" t="n">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="Z26" t="n">
         <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="AB26" t="n">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="AC26" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="AD26" t="n">
         <v>2.5</v>
       </c>
       <c r="AE26" t="inlineStr">
         <is>
-          <t>Line of targets take 10.00% more damage over 10.00 seconds (max 4.00 stacks)</t>
-        </is>
-      </c>
-      <c r="AF26" t="inlineStr"/>
+          <t>Rapidly regenerates life</t>
+        </is>
+      </c>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>Gives ideal income for the cost</t>
+        </is>
+      </c>
       <c r="AG26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Wrathwalker</t>
+          <t>Hellion</t>
         </is>
       </c>
       <c r="B27">
@@ -3443,16 +3443,16 @@
         <v/>
       </c>
       <c r="G27" t="n">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="H27" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="I27" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J27" t="n">
-        <v>17.5</v>
+        <v>15</v>
       </c>
       <c r="K27">
         <f>E27/G27</f>
@@ -3472,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
@@ -3484,14 +3484,14 @@
         <v>1</v>
       </c>
       <c r="T27" t="n">
-        <v>706</v>
+        <v>735</v>
       </c>
       <c r="U27" t="n">
         <v>0</v>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>Armored</t>
+          <t>Light</t>
         </is>
       </c>
       <c r="W27" t="n">
@@ -3499,20 +3499,20 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>Siege</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="Y27" t="n">
-        <v>6.9</v>
+        <v>4</v>
       </c>
       <c r="Z27" t="n">
         <v>1</v>
       </c>
       <c r="AA27" t="n">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="AB27" t="n">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="AC27" t="n">
         <v>1.1</v>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="AE27" t="inlineStr">
         <is>
-          <t>2x damage to Security Systems</t>
+          <t>Line of targets take 10.00% more damage over 10.00 seconds (max 4.00 stacks)</t>
         </is>
       </c>
       <c r="AF27" t="inlineStr"/>
@@ -3531,7 +3531,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Feederling</t>
+          <t>Wrathwalker</t>
         </is>
       </c>
       <c r="B28">
@@ -3555,16 +3555,16 @@
         <v/>
       </c>
       <c r="G28" t="n">
-        <v>600</v>
+        <v>440</v>
       </c>
       <c r="H28" t="n">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="I28" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J28" t="n">
-        <v>20</v>
+        <v>17.5</v>
       </c>
       <c r="K28">
         <f>E28/G28</f>
@@ -3575,7 +3575,7 @@
         <v/>
       </c>
       <c r="M28" t="n">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="N28" t="n">
         <v>1</v>
@@ -3596,14 +3596,14 @@
         <v>1</v>
       </c>
       <c r="T28" t="n">
-        <v>1218</v>
+        <v>706</v>
       </c>
       <c r="U28" t="n">
         <v>0</v>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Armored</t>
         </is>
       </c>
       <c r="W28" t="n">
@@ -3611,30 +3611,30 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Siege</t>
         </is>
       </c>
       <c r="Y28" t="n">
-        <v>2</v>
+        <v>6.9</v>
       </c>
       <c r="Z28" t="n">
         <v>1</v>
       </c>
       <c r="AA28" t="n">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="AB28" t="n">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="AC28" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="AD28" t="n">
         <v>2.5</v>
       </c>
       <c r="AE28" t="inlineStr">
         <is>
-          <t>Nearby melee allies gain 30.00% lifesteal to attacks (does not stack)</t>
+          <t>2x damage to Security Systems</t>
         </is>
       </c>
       <c r="AF28" t="inlineStr"/>
@@ -3643,7 +3643,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>High Templar</t>
+          <t>Feederling</t>
         </is>
       </c>
       <c r="B29">
@@ -3687,7 +3687,7 @@
         <v/>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="N29" t="n">
         <v>1</v>
@@ -3696,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
@@ -3708,45 +3708,45 @@
         <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>918</v>
+        <v>1218</v>
       </c>
       <c r="U29" t="n">
         <v>0</v>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>Light</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W29" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>Magic</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="Y29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z29" t="n">
         <v>1</v>
       </c>
       <c r="AA29" t="n">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="AB29" t="n">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="AD29" t="n">
         <v>2.5</v>
       </c>
       <c r="AE29" t="inlineStr">
         <is>
-          <t>One ally attacks and moves 20% faster (does not stack)</t>
+          <t>Nearby melee allies gain 30.00% lifesteal to attacks (does not stack)</t>
         </is>
       </c>
       <c r="AF29" t="inlineStr"/>
@@ -3755,7 +3755,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Broodlord</t>
+          <t>High Templar</t>
         </is>
       </c>
       <c r="B30">
@@ -3779,16 +3779,16 @@
         <v/>
       </c>
       <c r="G30" t="n">
-        <v>670</v>
+        <v>600</v>
       </c>
       <c r="H30" t="n">
-        <v>425</v>
+        <v>400</v>
       </c>
       <c r="I30" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J30" t="n">
-        <v>21.25</v>
+        <v>20</v>
       </c>
       <c r="K30">
         <f>E30/G30</f>
@@ -3799,7 +3799,7 @@
         <v/>
       </c>
       <c r="M30" t="n">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
         <v>1</v>
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -3820,45 +3820,45 @@
         <v>1</v>
       </c>
       <c r="T30" t="n">
-        <v>588</v>
+        <v>918</v>
       </c>
       <c r="U30" t="n">
         <v>0</v>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Light</t>
         </is>
       </c>
       <c r="W30" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>Piercing</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="Y30" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA30" t="n">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="AB30" t="n">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="AC30" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AD30" t="n">
         <v>2.5</v>
       </c>
       <c r="AE30" t="inlineStr">
         <is>
-          <t>Attacks spawn two broodlings</t>
+          <t>One ally attacks and moves 20% faster (does not stack)</t>
         </is>
       </c>
       <c r="AF30" t="inlineStr"/>
@@ -3867,7 +3867,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Banshee</t>
+          <t>Broodlord</t>
         </is>
       </c>
       <c r="B31">
@@ -3891,16 +3891,16 @@
         <v/>
       </c>
       <c r="G31" t="n">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="H31" t="n">
-        <v>450</v>
+        <v>425</v>
       </c>
       <c r="I31" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J31" t="n">
-        <v>22.5</v>
+        <v>21.25</v>
       </c>
       <c r="K31">
         <f>E31/G31</f>
@@ -3911,7 +3911,7 @@
         <v/>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="N31" t="n">
         <v>1</v>
@@ -3920,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q31" t="n">
         <v>0</v>
@@ -3932,14 +3932,14 @@
         <v>1</v>
       </c>
       <c r="T31" t="n">
-        <v>1294</v>
+        <v>588</v>
       </c>
       <c r="U31" t="n">
         <v>0</v>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>Light</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W31" t="n">
@@ -3947,30 +3947,30 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>Magic</t>
+          <t>Piercing</t>
         </is>
       </c>
       <c r="Y31" t="n">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="Z31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA31" t="n">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="AB31" t="n">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="AC31" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="AD31" t="n">
         <v>2.5</v>
       </c>
       <c r="AE31" t="inlineStr">
         <is>
-          <t>100% splash damage</t>
+          <t>Attacks spawn two broodlings</t>
         </is>
       </c>
       <c r="AF31" t="inlineStr"/>
@@ -3979,7 +3979,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Quillgore</t>
+          <t>Banshee</t>
         </is>
       </c>
       <c r="B32">
@@ -4003,16 +4003,16 @@
         <v/>
       </c>
       <c r="G32" t="n">
-        <v>500</v>
+        <v>680</v>
       </c>
       <c r="H32" t="n">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I32" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J32" t="n">
-        <v>25</v>
+        <v>22.5</v>
       </c>
       <c r="K32">
         <f>E32/G32</f>
@@ -4032,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -4044,14 +4044,14 @@
         <v>1</v>
       </c>
       <c r="T32" t="n">
-        <v>1758</v>
+        <v>1294</v>
       </c>
       <c r="U32" t="n">
         <v>0</v>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>Armored</t>
+          <t>Light</t>
         </is>
       </c>
       <c r="W32" t="n">
@@ -4059,30 +4059,30 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>Piercing</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="Y32" t="n">
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="Z32" t="n">
         <v>1</v>
       </c>
       <c r="AA32" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="AB32" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="AC32" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="AD32" t="n">
         <v>2.5</v>
       </c>
       <c r="AE32" t="inlineStr">
         <is>
-          <t>Gives ideal income for the cost</t>
+          <t>100% splash damage</t>
         </is>
       </c>
       <c r="AF32" t="inlineStr"/>
@@ -4091,7 +4091,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ultralisk</t>
+          <t>Quillgore</t>
         </is>
       </c>
       <c r="B33">
@@ -4115,16 +4115,16 @@
         <v/>
       </c>
       <c r="G33" t="n">
-        <v>620</v>
+        <v>500</v>
       </c>
       <c r="H33" t="n">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="I33" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J33" t="n">
-        <v>25.5</v>
+        <v>25</v>
       </c>
       <c r="K33">
         <f>E33/G33</f>
@@ -4147,7 +4147,7 @@
         <v>1</v>
       </c>
       <c r="Q33" t="n">
-        <v>185</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
         <v>1</v>
@@ -4156,14 +4156,14 @@
         <v>1</v>
       </c>
       <c r="T33" t="n">
-        <v>1510</v>
+        <v>1758</v>
       </c>
       <c r="U33" t="n">
         <v>0</v>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Armored</t>
         </is>
       </c>
       <c r="W33" t="n">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>Siege</t>
+          <t>Piercing</t>
         </is>
       </c>
       <c r="Y33" t="n">
@@ -4181,10 +4181,10 @@
         <v>1</v>
       </c>
       <c r="AA33" t="n">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="AB33" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="AC33" t="n">
         <v>1.3</v>
@@ -4194,20 +4194,16 @@
       </c>
       <c r="AE33" t="inlineStr">
         <is>
-          <t>Crushes the target and all units behind for 37.00 damage once every 2 attacks.</t>
-        </is>
-      </c>
-      <c r="AF33" t="inlineStr">
-        <is>
-          <t>Untargetable by abilities and takes no spell damage</t>
-        </is>
-      </c>
+          <t>Gives ideal income for the cost</t>
+        </is>
+      </c>
+      <c r="AF33" t="inlineStr"/>
       <c r="AG33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Hunterling</t>
+          <t>Ultralisk</t>
         </is>
       </c>
       <c r="B34">
@@ -4231,16 +4227,16 @@
         <v/>
       </c>
       <c r="G34" t="n">
-        <v>840</v>
+        <v>620</v>
       </c>
       <c r="H34" t="n">
-        <v>540</v>
+        <v>510</v>
       </c>
       <c r="I34" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J34" t="n">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="K34">
         <f>E34/G34</f>
@@ -4254,7 +4250,7 @@
         <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>1.18</v>
+        <v>1</v>
       </c>
       <c r="O34" t="n">
         <v>0</v>
@@ -4263,7 +4259,7 @@
         <v>1</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="R34" t="n">
         <v>1</v>
@@ -4272,14 +4268,14 @@
         <v>1</v>
       </c>
       <c r="T34" t="n">
-        <v>3075</v>
+        <v>1510</v>
       </c>
       <c r="U34" t="n">
         <v>0</v>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W34" t="n">
@@ -4287,7 +4283,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Siege</t>
         </is>
       </c>
       <c r="Y34" t="n">
@@ -4297,29 +4293,33 @@
         <v>1</v>
       </c>
       <c r="AA34" t="n">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="AB34" t="n">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="AC34" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="AD34" t="n">
         <v>2.5</v>
       </c>
       <c r="AE34" t="inlineStr">
         <is>
-          <t>Jumps towards an enemy unit, disorienting nearby enemies and reducing their damage output by 30.00%.</t>
-        </is>
-      </c>
-      <c r="AF34" t="inlineStr"/>
+          <t>Crushes the target and all units behind for 37.00 damage once every 2 attacks.</t>
+        </is>
+      </c>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>Untargetable by abilities and takes no spell damage</t>
+        </is>
+      </c>
       <c r="AG34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Shadow Templar</t>
+          <t>Hunterling</t>
         </is>
       </c>
       <c r="B35">
@@ -4343,16 +4343,16 @@
         <v/>
       </c>
       <c r="G35" t="n">
-        <v>880</v>
+        <v>840</v>
       </c>
       <c r="H35" t="n">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="I35" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J35" t="n">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="K35">
         <f>E35/G35</f>
@@ -4366,7 +4366,7 @@
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>1</v>
+        <v>1.18</v>
       </c>
       <c r="O35" t="n">
         <v>0</v>
@@ -4384,14 +4384,14 @@
         <v>1</v>
       </c>
       <c r="T35" t="n">
-        <v>1765</v>
+        <v>3075</v>
       </c>
       <c r="U35" t="n">
         <v>0</v>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>Armored</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="W35" t="n">
@@ -4409,20 +4409,20 @@
         <v>1</v>
       </c>
       <c r="AA35" t="n">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="AB35" t="n">
-        <v>186</v>
+        <v>36</v>
       </c>
       <c r="AC35" t="n">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="AD35" t="n">
         <v>2.5</v>
       </c>
       <c r="AE35" t="inlineStr">
         <is>
-          <t>Grants nearby allies significant resistance to movement speed debuffs.</t>
+          <t>Jumps towards an enemy unit, disorienting nearby enemies and reducing their damage output by 30.00%.</t>
         </is>
       </c>
       <c r="AF35" t="inlineStr"/>
@@ -4431,7 +4431,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Aberration Pulverizer</t>
+          <t>Shadow Templar</t>
         </is>
       </c>
       <c r="B36">
@@ -4455,16 +4455,16 @@
         <v/>
       </c>
       <c r="G36" t="n">
-        <v>900</v>
+        <v>880</v>
       </c>
       <c r="H36" t="n">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="I36" t="n">
         <v>11</v>
       </c>
       <c r="J36" t="n">
-        <v>28</v>
+        <v>27.5</v>
       </c>
       <c r="K36">
         <f>E36/G36</f>
@@ -4484,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q36" t="n">
         <v>0</v>
@@ -4496,14 +4496,14 @@
         <v>1</v>
       </c>
       <c r="T36" t="n">
-        <v>1800</v>
+        <v>1765</v>
       </c>
       <c r="U36" t="n">
         <v>0</v>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Armored</t>
         </is>
       </c>
       <c r="W36" t="n">
@@ -4511,30 +4511,30 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>Siege</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="Y36" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="Z36" t="n">
         <v>1</v>
       </c>
       <c r="AA36" t="n">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="AB36" t="n">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="AC36" t="n">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="AD36" t="n">
         <v>2.5</v>
       </c>
       <c r="AE36" t="inlineStr">
         <is>
-          <t>Attacks all enemies within reach</t>
+          <t>Grants nearby allies significant resistance to movement speed debuffs.</t>
         </is>
       </c>
       <c r="AF36" t="inlineStr"/>
@@ -4543,7 +4543,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Thor</t>
+          <t>Aberration Pulverizer</t>
         </is>
       </c>
       <c r="B37">
@@ -4567,16 +4567,16 @@
         <v/>
       </c>
       <c r="G37" t="n">
-        <v>960</v>
+        <v>900</v>
       </c>
       <c r="H37" t="n">
-        <v>600</v>
+        <v>560</v>
       </c>
       <c r="I37" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J37" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K37">
         <f>E37/G37</f>
@@ -4593,10 +4593,10 @@
         <v>1</v>
       </c>
       <c r="O37" t="n">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q37" t="n">
         <v>0</v>
@@ -4608,14 +4608,14 @@
         <v>1</v>
       </c>
       <c r="T37" t="n">
-        <v>1512</v>
+        <v>1800</v>
       </c>
       <c r="U37" t="n">
         <v>0</v>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W37" t="n">
@@ -4623,43 +4623,39 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>Piercing</t>
+          <t>Siege</t>
         </is>
       </c>
       <c r="Y37" t="n">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="Z37" t="n">
         <v>1</v>
       </c>
       <c r="AA37" t="n">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="AB37" t="n">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="AC37" t="n">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="AD37" t="n">
         <v>2.5</v>
       </c>
       <c r="AE37" t="inlineStr">
         <is>
-          <t>Target attacks and moves 20% slower while losing 65 HP/s for 6 seconds (does not stack)</t>
-        </is>
-      </c>
-      <c r="AF37" t="inlineStr">
-        <is>
-          <t>Untargetable by abilities and takes no spell damage</t>
-        </is>
-      </c>
+          <t>Attacks all enemies within reach</t>
+        </is>
+      </c>
+      <c r="AF37" t="inlineStr"/>
       <c r="AG37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Hybrid Dominator</t>
+          <t>Thor</t>
         </is>
       </c>
       <c r="B38">
@@ -4683,16 +4679,16 @@
         <v/>
       </c>
       <c r="G38" t="n">
-        <v>1340</v>
+        <v>960</v>
       </c>
       <c r="H38" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="I38" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J38" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="K38">
         <f>E38/G38</f>
@@ -4709,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="P38" t="n">
         <v>1</v>
@@ -4724,50 +4720,50 @@
         <v>1</v>
       </c>
       <c r="T38" t="n">
-        <v>2332</v>
+        <v>1512</v>
       </c>
       <c r="U38" t="n">
         <v>0</v>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>Massive</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="W38" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>Magic</t>
+          <t>Piercing</t>
         </is>
       </c>
       <c r="Y38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z38" t="n">
         <v>1</v>
       </c>
       <c r="AA38" t="n">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="AB38" t="n">
-        <v>230</v>
+        <v>184</v>
       </c>
       <c r="AC38" t="n">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="AD38" t="n">
         <v>2.5</v>
       </c>
       <c r="AE38" t="inlineStr">
         <is>
-          <t>Steals 0.50 energy/s from enemies within 10.00 range (max -5.00 energy/s).</t>
+          <t>Target attacks and moves 20% slower while losing 65 HP/s for 6 seconds (does not stack)</t>
         </is>
       </c>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>Strips 20.00 energy and 200.00 shields from foes within 10.00 range for 100 energy.</t>
+          <t>Untargetable by abilities and takes no spell damage</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -4775,7 +4771,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Flame Behemoth</t>
+          <t>Hybrid Dominator</t>
         </is>
       </c>
       <c r="B39">
@@ -4799,16 +4795,16 @@
         <v/>
       </c>
       <c r="G39" t="n">
-        <v>1720</v>
+        <v>1340</v>
       </c>
       <c r="H39" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="I39" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J39" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K39">
         <f>E39/G39</f>
@@ -4825,7 +4821,7 @@
         <v>1</v>
       </c>
       <c r="O39" t="n">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="P39" t="n">
         <v>1</v>
@@ -4840,22 +4836,22 @@
         <v>1</v>
       </c>
       <c r="T39" t="n">
-        <v>2458</v>
+        <v>2332</v>
       </c>
       <c r="U39" t="n">
         <v>0</v>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Massive</t>
         </is>
       </c>
       <c r="W39" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>Piercing</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="Y39" t="n">
@@ -4865,25 +4861,25 @@
         <v>1</v>
       </c>
       <c r="AA39" t="n">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="AB39" t="n">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="AC39" t="n">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="AD39" t="n">
         <v>2.5</v>
       </c>
       <c r="AE39" t="inlineStr">
         <is>
-          <t>While 5+ foes are within attack range, inflicts 150.00 damage/s to 5.00 enemies within 5.00 range (does not stack).</t>
+          <t>Steals 0.50 energy/s from enemies within 10.00 range (max -5.00 energy/s).</t>
         </is>
       </c>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>Not affected by most stun abilities.</t>
+          <t>Strips 20.00 energy and 200.00 shields from foes within 10.00 range for 100 energy.</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -4891,7 +4887,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Tyrannozor</t>
+          <t>Flame Behemoth</t>
         </is>
       </c>
       <c r="B40">
@@ -4915,16 +4911,16 @@
         <v/>
       </c>
       <c r="G40" t="n">
-        <v>1900</v>
+        <v>1720</v>
       </c>
       <c r="H40" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="I40" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J40" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K40">
         <f>E40/G40</f>
@@ -4941,7 +4937,7 @@
         <v>1</v>
       </c>
       <c r="O40" t="n">
-        <v>151</v>
+        <v>450</v>
       </c>
       <c r="P40" t="n">
         <v>1</v>
@@ -4956,14 +4952,14 @@
         <v>1</v>
       </c>
       <c r="T40" t="n">
-        <v>6050</v>
+        <v>2458</v>
       </c>
       <c r="U40" t="n">
         <v>0</v>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>Biological</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="W40" t="n">
@@ -4971,34 +4967,150 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Piercing</t>
         </is>
       </c>
       <c r="Y40" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="Z40" t="n">
         <v>1</v>
       </c>
       <c r="AA40" t="n">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="AB40" t="n">
-        <v>175</v>
+        <v>258</v>
       </c>
       <c r="AC40" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="AD40" t="n">
         <v>2.5</v>
       </c>
       <c r="AE40" t="inlineStr">
         <is>
+          <t>While 5+ foes are within attack range, inflicts 150.00 damage/s to 5.00 enemies within 5.00 range (does not stack).</t>
+        </is>
+      </c>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>Not affected by most stun abilities.</t>
+        </is>
+      </c>
+      <c r="AG40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Tyrannozor</t>
+        </is>
+      </c>
+      <c r="B41">
+        <f>D41*C41</f>
+        <v/>
+      </c>
+      <c r="C41">
+        <f>K41/AVERAGE(K2:K65535)</f>
+        <v/>
+      </c>
+      <c r="D41">
+        <f>L41/AVERAGE(L2:L65535)</f>
+        <v/>
+      </c>
+      <c r="E41">
+        <f>N41*(T41+U41+M41)</f>
+        <v/>
+      </c>
+      <c r="F41">
+        <f>P41*(O41+Z41*R41*((AA41+AB41)/2+Q41)/(AC41/S41))</f>
+        <v/>
+      </c>
+      <c r="G41" t="n">
+        <v>1900</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1100</v>
+      </c>
+      <c r="I41" t="n">
+        <v>15</v>
+      </c>
+      <c r="J41" t="n">
+        <v>55</v>
+      </c>
+      <c r="K41">
+        <f>E41/G41</f>
+        <v/>
+      </c>
+      <c r="L41">
+        <f>F41/G41</f>
+        <v/>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" t="n">
+        <v>151</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1</v>
+      </c>
+      <c r="S41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T41" t="n">
+        <v>6050</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>Biological</t>
+        </is>
+      </c>
+      <c r="W41" t="n">
+        <v>0</v>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="Y41" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>152</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>175</v>
+      </c>
+      <c r="AC41" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AD41" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
           <t>Reflects 180.00% of damage taken back to the attacker (minimum 90.00 damage).</t>
         </is>
       </c>
-      <c r="AF40" t="inlineStr"/>
-      <c r="AG40" t="inlineStr"/>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>